<commit_message>
add the mouse move
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_cb7\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{9B3A6766-299D-4165-B24B-D96F491643DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC5D4DCA-CD9F-4513-AA9E-171E7A5EE785}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{9B3A6766-299D-4165-B24B-D96F491643DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BA3EDAD-08C2-4B11-BF29-313A1F846F8F}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,7 +371,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -414,7 +414,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -433,7 +433,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>